<commit_message>
organização finalizada do sumário.
</commit_message>
<xml_diff>
--- a/documentação/analise de benchmarking.xlsx
+++ b/documentação/analise de benchmarking.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t xml:space="preserve">GRUPO: Kévin</t>
   </si>
@@ -30,6 +30,15 @@
   <si>
     <t xml:space="preserve">ANÁLISE DE BENCHMARKING - AVALIAÇÃO DE 1 A 5</t>
   </si>
+  <si>
+    <t xml:space="preserve">Sudoku</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Math Master</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cálculo Mental</t>
+  </si>
 </sst>
 </file>
 
@@ -38,7 +47,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -92,6 +101,11 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Roboto"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -317,7 +331,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v/>
+                  <c:v>Sudoku</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -401,7 +415,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v/>
+                  <c:v>Math Master</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -485,7 +499,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v/>
+                  <c:v>Cálculo Mental</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -560,13 +574,13 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="4319838"/>
-        <c:axId val="53634125"/>
+        <c:axId val="84513315"/>
+        <c:axId val="29706926"/>
       </c:radarChart>
       <c:catAx>
-        <c:axId val="4319838"/>
+        <c:axId val="84513315"/>
         <c:scaling>
-          <c:orientation val="maxMin"/>
+          <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -597,14 +611,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="53634125"/>
+        <c:crossAx val="29706926"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="53634125"/>
+        <c:axId val="29706926"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -647,7 +661,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="4319838"/>
+        <c:crossAx val="84513315"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -695,9 +709,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>142560</xdr:colOff>
+      <xdr:colOff>142200</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>56880</xdr:rowOff>
+      <xdr:rowOff>56520</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -705,8 +719,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="1895400" y="2523960"/>
-        <a:ext cx="5714640" cy="3533400"/>
+        <a:off x="1876320" y="2523960"/>
+        <a:ext cx="5618880" cy="3533040"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -727,16 +741,16 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
+      <selection pane="topLeft" activeCell="E5" activeCellId="0" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="14.1734693877551"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="25.1071428571429"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="24.1632653061224"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="28.2142857142857"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="14.1734693877551"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="13.9030612244898"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="24.8367346938776"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="23.7602040816327"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="27.8061224489796"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="13.9030612244898"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -765,9 +779,15 @@
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B5" s="3"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
+      <c r="C5" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B6" s="5"/>

</xml_diff>

<commit_message>
feito a análise de benchmarking e começando a desenvolver pareto.
</commit_message>
<xml_diff>
--- a/documentação/analise de benchmarking.xlsx
+++ b/documentação/analise de benchmarking.xlsx
@@ -20,9 +20,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
-  <si>
-    <t xml:space="preserve">GRUPO: Kévin</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+  <si>
+    <t xml:space="preserve">GRUPO: Kévin Vieira Gomes Guimarães</t>
   </si>
   <si>
     <t xml:space="preserve">TEMÁTICA: Desafio matématico com IA</t>
@@ -34,10 +34,25 @@
     <t xml:space="preserve">Sudoku</t>
   </si>
   <si>
-    <t xml:space="preserve">Math Master</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cálculo Mental</t>
+    <t xml:space="preserve">Calculadora Quebrada</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aritmética com Cartas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">interface</t>
+  </si>
+  <si>
+    <t xml:space="preserve">conteúdo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dinamica</t>
+  </si>
+  <si>
+    <t xml:space="preserve">componentes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cores</t>
   </si>
 </sst>
 </file>
@@ -364,19 +379,19 @@
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v/>
+                  <c:v>interface</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v/>
+                  <c:v>conteúdo</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v/>
+                  <c:v>dinamica</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v/>
+                  <c:v>componentes</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v/>
+                  <c:v>cores</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -388,19 +403,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v/>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v/>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v/>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v/>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v/>
+                  <c:v>5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -415,7 +430,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Math Master</c:v>
+                  <c:v>Calculadora Quebrada</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -448,19 +463,19 @@
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v/>
+                  <c:v>interface</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v/>
+                  <c:v>conteúdo</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v/>
+                  <c:v>dinamica</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v/>
+                  <c:v>componentes</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v/>
+                  <c:v>cores</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -472,19 +487,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v/>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v/>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v/>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v/>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v/>
+                  <c:v>3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -499,7 +514,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Cálculo Mental</c:v>
+                  <c:v>Aritmética com Cartas</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -532,19 +547,19 @@
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v/>
+                  <c:v>interface</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v/>
+                  <c:v>conteúdo</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v/>
+                  <c:v>dinamica</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v/>
+                  <c:v>componentes</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v/>
+                  <c:v>cores</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -556,31 +571,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v/>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v/>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v/>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v/>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v/>
+                  <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="84513315"/>
-        <c:axId val="29706926"/>
+        <c:axId val="60590849"/>
+        <c:axId val="6972813"/>
       </c:radarChart>
       <c:catAx>
-        <c:axId val="84513315"/>
+        <c:axId val="60590849"/>
         <c:scaling>
-          <c:orientation val="minMax"/>
+          <c:orientation val="maxMin"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -611,14 +626,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="29706926"/>
+        <c:crossAx val="6972813"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="29706926"/>
+        <c:axId val="6972813"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -661,7 +676,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="84513315"/>
+        <c:crossAx val="60590849"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -702,16 +717,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>895320</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>123840</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>46080</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>142200</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>56520</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>928440</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>188640</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -719,8 +734,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="1876320" y="2523960"/>
-        <a:ext cx="5618880" cy="3533040"/>
+        <a:off x="0" y="2046240"/>
+        <a:ext cx="13577400" cy="6543360"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -740,17 +755,17 @@
   </sheetPr>
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E5" activeCellId="0" sqref="E5"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D31" activeCellId="0" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="13.9030612244898"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="24.8367346938776"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="23.7602040816327"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="27.8061224489796"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="13.9030612244898"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.8928571428571"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.6785714285714"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="26.8622448979592"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="13.2295918367347"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -790,34 +805,74 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B6" s="5"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
+      <c r="B6" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="6" t="n">
+        <v>5</v>
+      </c>
+      <c r="D6" s="6" t="n">
+        <v>4</v>
+      </c>
+      <c r="E6" s="6" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B7" s="5"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
+      <c r="B7" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="D7" s="6" t="n">
+        <v>3</v>
+      </c>
+      <c r="E7" s="6" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B8" s="5"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
+      <c r="B8" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="D8" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="E8" s="6" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B9" s="5"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
+      <c r="B9" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="6" t="n">
+        <v>3</v>
+      </c>
+      <c r="D9" s="6" t="n">
+        <v>4</v>
+      </c>
+      <c r="E9" s="6" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B10" s="5"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
+      <c r="B10" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="6" t="n">
+        <v>5</v>
+      </c>
+      <c r="D10" s="6" t="n">
+        <v>3</v>
+      </c>
+      <c r="E10" s="6" t="n">
+        <v>2</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>